<commit_message>
update in mar 28th
</commit_message>
<xml_diff>
--- a/templates/Excel/ST1_Line_Rejection.xlsx
+++ b/templates/Excel/ST1_Line_Rejection.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,16 +518,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-02-22T18:34</t>
+          <t>2025-03-26T12:33</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SHIFT_2</t>
+          <t>SHIFT_1</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -561,7 +561,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>Suriya</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-02-23T12:56</t>
+          <t>2025-03-27T12:22</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -587,58 +587,58 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>TEST</t>
+          <t>Suri</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>suri</t>
+          <t>Suri</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>suri</t>
+          <t>Suri</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-02-24T12:54</t>
+          <t>2025-03-27T12:31</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -646,74 +646,134 @@
           <t>SHIFT_1</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-03-27T12:36</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SHIFT_1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>suriya</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>suriya</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>suriya</t>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>t</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
data and shift change
</commit_message>
<xml_diff>
--- a/templates/Excel/ST1_Line_Rejection.xlsx
+++ b/templates/Excel/ST1_Line_Rejection.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -706,74 +706,238 @@
           <t>SHIFT_1</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-03-31 14:29:35</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SHIFT_1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>t</t>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>